<commit_message>
Next step:choice the data of AT24-1.0
</commit_message>
<xml_diff>
--- a/Data/ElementTreatmentEl-UTS/ElementTreatmentEl-UTS.xlsx
+++ b/Data/ElementTreatmentEl-UTS/ElementTreatmentEl-UTS.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MLDesignAl\TheFinal\Data\ElementTreatmentEl-UTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63205560-9572-47A4-8922-DE2690DA50AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A507E19-8131-4391-99A0-A10729B571E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2172" yWindow="132" windowWidth="19320" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="996" yWindow="672" windowWidth="20712" windowHeight="10584" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$S$1:$S$1293</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$M$1:$M$527</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -109,6 +109,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -220,7 +223,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="百分比" xfId="1" builtinId="5"/>
@@ -504,8 +507,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W527"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="A526" sqref="A526:Q527"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A514" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U531" sqref="U531"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -37791,26 +37795,196 @@
         <v>296</v>
       </c>
     </row>
+    <row r="526" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A526">
+        <f>MIN(A2:A525)</f>
+        <v>0</v>
+      </c>
+      <c r="B526">
+        <f t="shared" ref="B526:U526" si="0">MIN(B2:B525)</f>
+        <v>0</v>
+      </c>
+      <c r="C526">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D526">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E526">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F526">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G526">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H526">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I526">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J526">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K526">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L526">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M526">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N526">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O526">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P526">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q526">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R526">
+        <f t="shared" si="0"/>
+        <v>83.55</v>
+      </c>
+      <c r="S526">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+      <c r="T526">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="U526">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V526">
+        <f t="shared" ref="V526:W526" si="1">MIN(V2:V525)</f>
+        <v>0.5</v>
+      </c>
+      <c r="W526">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+    </row>
     <row r="527" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A527" s="10"/>
-      <c r="B527" s="10"/>
-      <c r="C527" s="10"/>
-      <c r="D527" s="10"/>
-      <c r="E527" s="10"/>
-      <c r="F527" s="10"/>
-      <c r="G527" s="10"/>
-      <c r="H527" s="10"/>
-      <c r="I527" s="10"/>
-      <c r="J527" s="10"/>
-      <c r="K527" s="10"/>
-      <c r="L527" s="10"/>
-      <c r="M527" s="10"/>
-      <c r="N527" s="10"/>
-      <c r="O527" s="10"/>
-      <c r="P527" s="10"/>
-      <c r="Q527" s="10"/>
+      <c r="A527" s="10">
+        <f>MAX(A2:A525)</f>
+        <v>12.25</v>
+      </c>
+      <c r="B527" s="10">
+        <f t="shared" ref="B527:U527" si="2">MAX(B2:B525)</f>
+        <v>1.3</v>
+      </c>
+      <c r="C527" s="10">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="D527" s="10">
+        <f t="shared" si="2"/>
+        <v>1.31</v>
+      </c>
+      <c r="E527" s="10">
+        <f t="shared" si="2"/>
+        <v>3.64</v>
+      </c>
+      <c r="F527" s="10">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="G527" s="10">
+        <f t="shared" si="2"/>
+        <v>8.6</v>
+      </c>
+      <c r="H527" s="10">
+        <f t="shared" si="2"/>
+        <v>0.158</v>
+      </c>
+      <c r="I527" s="10">
+        <f t="shared" si="2"/>
+        <v>2.5</v>
+      </c>
+      <c r="J527" s="10">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="K527" s="10">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="L527" s="10">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M527" s="10">
+        <f t="shared" si="2"/>
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="N527" s="10">
+        <f t="shared" si="2"/>
+        <v>0.48</v>
+      </c>
+      <c r="O527" s="10">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
+      <c r="P527" s="10">
+        <f t="shared" si="2"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="Q527" s="10">
+        <f t="shared" si="2"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="R527" s="10">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="S527" s="10">
+        <f t="shared" si="2"/>
+        <v>590</v>
+      </c>
+      <c r="T527" s="10">
+        <f t="shared" si="2"/>
+        <v>345</v>
+      </c>
+      <c r="U527" s="10">
+        <f t="shared" si="2"/>
+        <v>1440</v>
+      </c>
+      <c r="V527" s="10">
+        <f t="shared" ref="V527:W527" si="3">MAX(V2:V525)</f>
+        <v>47.9</v>
+      </c>
+      <c r="W527" s="10">
+        <f t="shared" si="3"/>
+        <v>710</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="M1:M527" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>